<commit_message>
update all plot results
</commit_message>
<xml_diff>
--- a/singleVis/plot/plot_results/PPR.xlsx
+++ b/singleVis/plot/plot_results/PPR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,14 +486,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>DVI(Train)</t>
         </is>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.994</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="3">
@@ -517,14 +517,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>DVI(Test)</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.985</v>
+        <v>0.9684999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -548,14 +548,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>DVI(Train)</t>
         </is>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.991</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="5">
@@ -579,14 +579,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>DVI(Test)</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.989</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="6">
@@ -610,7 +610,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>DVI(Train)</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>DVI(Test)</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -672,14 +672,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>TimeVis(Train)</t>
         </is>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.9644999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -703,14 +703,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>TimeVis(Test)</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9389999999999999</v>
+        <v>0.9615</v>
       </c>
     </row>
     <row r="10">
@@ -734,14 +734,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>TimeVis(Train)</t>
         </is>
       </c>
       <c r="F10" t="n">
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.976</v>
+        <v>0.9944999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -765,14 +765,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>TimeVis(Test)</t>
         </is>
       </c>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.973</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="12">
@@ -796,14 +796,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>TimeVis(Train)</t>
         </is>
       </c>
       <c r="F12" t="n">
         <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -827,14 +827,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>TimeVis(Test)</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>0.992</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="14">
@@ -843,12 +843,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>fmnist</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -858,14 +858,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>DeepDebugger(Train)</t>
         </is>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9340000000000001</v>
+        <v>0.9575</v>
       </c>
     </row>
     <row r="15">
@@ -874,12 +874,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>fmnist</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -889,14 +889,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>DeepDebugger(Test)</t>
         </is>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.923</v>
+        <v>0.955</v>
       </c>
     </row>
     <row r="16">
@@ -905,12 +905,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>fmnist</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -920,14 +920,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>DeepDebugger(Train)</t>
         </is>
       </c>
       <c r="F16" t="n">
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0.995</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="17">
@@ -936,12 +936,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>fmnist</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -951,14 +951,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>DeepDebugger(Test)</t>
         </is>
       </c>
       <c r="F17" t="n">
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0.981</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="18">
@@ -967,12 +967,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>fmnist</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -982,14 +982,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>DeepDebugger(Train)</t>
         </is>
       </c>
       <c r="F18" t="n">
         <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>0.997</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -998,12 +998,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>fmnist</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1013,14 +1013,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>DeepDebugger(Test)</t>
         </is>
       </c>
       <c r="F19" t="n">
         <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>0.978</v>
+        <v>0.9975000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DVI</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1044,14 +1044,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>DVI(Train)</t>
         </is>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.836</v>
+        <v>0.8605</v>
       </c>
     </row>
     <row r="21">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DVI</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1075,14 +1075,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>DVI(Test)</t>
         </is>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="22">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DVI</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1106,14 +1106,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>DVI(Train)</t>
         </is>
       </c>
       <c r="F22" t="n">
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>0.999</v>
+        <v>0.9245000000000001</v>
       </c>
     </row>
     <row r="23">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DVI</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1137,14 +1137,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>DVI(Test)</t>
         </is>
       </c>
       <c r="F23" t="n">
         <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>0.987</v>
+        <v>0.9195</v>
       </c>
     </row>
     <row r="24">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DVI</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1168,14 +1168,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>DVI(Train)</t>
         </is>
       </c>
       <c r="F24" t="n">
         <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0.9550000000000001</v>
       </c>
     </row>
     <row r="25">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DVI</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1199,14 +1199,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>DVI(Test)</t>
         </is>
       </c>
       <c r="F25" t="n">
         <v>2</v>
       </c>
       <c r="G25" t="n">
-        <v>0.987</v>
+        <v>0.9455</v>
       </c>
     </row>
     <row r="26">
@@ -1215,12 +1215,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>TimeVis</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1230,14 +1230,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>TimeVis(Train)</t>
         </is>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0.913</v>
+        <v>0.841</v>
       </c>
     </row>
     <row r="27">
@@ -1246,12 +1246,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>TimeVis</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1261,14 +1261,14 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>TimeVis(Test)</t>
         </is>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.903</v>
+        <v>0.8315</v>
       </c>
     </row>
     <row r="28">
@@ -1277,12 +1277,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>TimeVis</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1292,14 +1292,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>TimeVis(Train)</t>
         </is>
       </c>
       <c r="F28" t="n">
         <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>0.9330000000000001</v>
+        <v>0.9624999999999999</v>
       </c>
     </row>
     <row r="29">
@@ -1308,12 +1308,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>TimeVis</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1323,14 +1323,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>TimeVis(Test)</t>
         </is>
       </c>
       <c r="F29" t="n">
         <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>0.912</v>
+        <v>0.953</v>
       </c>
     </row>
     <row r="30">
@@ -1339,12 +1339,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>TimeVis</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1354,14 +1354,14 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>DVI-Train</t>
+          <t>TimeVis(Train)</t>
         </is>
       </c>
       <c r="F30" t="n">
         <v>2</v>
       </c>
       <c r="G30" t="n">
-        <v>0.968</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="31">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>DVI</t>
+          <t>TimeVis</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1385,14 +1385,14 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>DVI-Test</t>
+          <t>TimeVis(Test)</t>
         </is>
       </c>
       <c r="F31" t="n">
         <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>0.93</v>
+        <v>0.978</v>
       </c>
     </row>
     <row r="32">
@@ -1401,12 +1401,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1416,14 +1416,14 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>DeepDebugger(Train)</t>
         </is>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0.842</v>
+        <v>0.8765000000000001</v>
       </c>
     </row>
     <row r="33">
@@ -1432,12 +1432,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1447,14 +1447,14 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>DeepDebugger(Test)</t>
         </is>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.841</v>
+        <v>0.8714999999999999</v>
       </c>
     </row>
     <row r="34">
@@ -1463,12 +1463,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1478,14 +1478,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>DeepDebugger(Train)</t>
         </is>
       </c>
       <c r="F34" t="n">
         <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>0.968</v>
+        <v>0.9795</v>
       </c>
     </row>
     <row r="35">
@@ -1494,12 +1494,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1509,14 +1509,14 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>DeepDebugger(Test)</t>
         </is>
       </c>
       <c r="F35" t="n">
         <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>0.953</v>
+        <v>0.972</v>
       </c>
     </row>
     <row r="36">
@@ -1525,12 +1525,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1540,14 +1540,14 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>TimeVis-Train</t>
+          <t>DeepDebugger(Train)</t>
         </is>
       </c>
       <c r="F36" t="n">
         <v>2</v>
       </c>
       <c r="G36" t="n">
-        <v>0.997</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="37">
@@ -1556,12 +1556,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>cifar10</t>
+          <t>fmnist</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TimeVis</t>
+          <t>DeepDebugger</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1571,14 +1571,572 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>TimeVis-Test</t>
+          <t>DeepDebugger(Test)</t>
         </is>
       </c>
       <c r="F37" t="n">
         <v>2</v>
       </c>
       <c r="G37" t="n">
-        <v>0.977</v>
+        <v>0.981</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>DVI</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>DVI(Train)</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.3735</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>DVI</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>DVI(Test)</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.369</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>DVI</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>DVI(Train)</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.8815</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>DVI</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>DVI(Test)</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.8785000000000001</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>DVI</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>DVI(Train)</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.966</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>DVI</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>DVI(Test)</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.9445</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>TimeVis</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>TimeVis(Train)</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.5044999999999999</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>TimeVis</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>TimeVis(Test)</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.5095000000000001</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>TimeVis</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>TimeVis(Train)</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.9370000000000001</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>TimeVis</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>TimeVis(Test)</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.931</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>TimeVis</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>TimeVis(Train)</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.9904999999999999</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>TimeVis</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>TimeVis(Test)</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.9775</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>DeepDebugger</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>DeepDebugger(Train)</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>DeepDebugger</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>DeepDebugger(Test)</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.6274999999999999</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>DeepDebugger</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>DeepDebugger(Train)</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.946</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>DeepDebugger</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>DeepDebugger(Test)</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.9424999999999999</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>DeepDebugger</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>DeepDebugger(Train)</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>2</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.9915</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>cifar10</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>DeepDebugger</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>DeepDebugger(Test)</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>2</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>